<commit_message>
Update how the facebook event is added
</commit_message>
<xml_diff>
--- a/swing_devils_vol.xlsx
+++ b/swing_devils_vol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedot\Documents\Python Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedot\Documents\Python Scripts\Swing-Devils-Volunteer-Randomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A173D247-061A-4497-881A-5CDF849E7B9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB38DFF-B65F-4AFD-9641-4E43DD77C6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{E81735BB-92FD-42FD-BF1A-60ACFAD3000F}"/>
   </bookViews>
@@ -481,7 +481,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -742,7 +742,9 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
change Doty to Kyle
</commit_message>
<xml_diff>
--- a/swing_devils_vol.xlsx
+++ b/swing_devils_vol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedot\Documents\Python Scripts\Swing-Devils-Volunteer-Randomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C15B0F-FED9-452A-9960-AC357CF2E449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7369134-7BE7-4411-8F91-EBBA115C24BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{E81735BB-92FD-42FD-BF1A-60ACFAD3000F}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>Second Friday</t>
   </si>
   <si>
-    <t>Doty</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Taylor</t>
+  </si>
+  <si>
+    <t>Kyle</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -546,7 +546,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -554,14 +554,14 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="2">
@@ -569,12 +569,12 @@
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -582,47 +582,47 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L3" s="2">
         <v>1</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" s="2">
         <v>0</v>
@@ -632,27 +632,27 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" s="2">
         <v>3</v>
@@ -662,29 +662,29 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L6" s="2">
         <v>4</v>
@@ -694,43 +694,43 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" s="2">
         <v>3</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -747,70 +747,70 @@
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L9" s="2">
         <v>3</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -822,39 +822,39 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L11" s="2">
         <v>5</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -870,35 +870,35 @@
         <v>0</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L13" s="2">
         <v>4</v>

</xml_diff>

<commit_message>
March first week update
</commit_message>
<xml_diff>
--- a/swing_devils_vol.xlsx
+++ b/swing_devils_vol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedot\Documents\Python Scripts\Swing-Devils-Volunteer-Randomizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle Doty\Documents\Python Scripts\Swing-Devils-Volunteer-Randomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBA7D96-6CA7-4A30-AFAA-8174DB8CD3D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ACA61D-CA65-422A-B826-E3B46C886E88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{E81735BB-92FD-42FD-BF1A-60ACFAD3000F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E81735BB-92FD-42FD-BF1A-60ACFAD3000F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -141,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,20 +149,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,60 +502,60 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.86328125" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.06640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -544,25 +565,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4">
         <v>5</v>
       </c>
       <c r="M2" s="1"/>
@@ -570,23 +591,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="4">
         <v>1</v>
       </c>
       <c r="M3" s="1"/>
@@ -594,123 +615,137 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="5">
         <v>1</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="4">
         <v>3</v>
       </c>
-      <c r="M5" s="3"/>
+      <c r="M5" s="2"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="2">
-        <v>4</v>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="2">
-        <v>3</v>
-      </c>
-      <c r="M7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2"/>
       <c r="N7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4">
         <v>0</v>
       </c>
       <c r="M8" s="1"/>
@@ -718,35 +753,35 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="4">
         <v>3</v>
       </c>
       <c r="M9" s="1"/>
@@ -754,79 +789,81 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="2">
-        <v>2</v>
-      </c>
-      <c r="M10" s="3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
         <v>43804</v>
       </c>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="4">
         <v>5</v>
       </c>
-      <c r="M11" s="3"/>
+      <c r="M11" s="2"/>
       <c r="N11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="4">
         <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
@@ -836,30 +873,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="2">
-        <v>4</v>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4">
+        <v>0</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>

</xml_diff>

<commit_message>
make it so that each person can only do 1 thing per month
</commit_message>
<xml_diff>
--- a/swing_devils_vol.xlsx
+++ b/swing_devils_vol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle Doty\Documents\Python Scripts\Swing-Devils-Volunteer-Randomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077EFAE7-2BD9-419A-A36A-0F9A5DCCD980}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67443F31-1A0B-4D1A-A8BC-959752352F3B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E81735BB-92FD-42FD-BF1A-60ACFAD3000F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -484,7 +484,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,15 +540,9 @@
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
@@ -596,9 +590,7 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -695,7 +687,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
@@ -756,7 +748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -777,7 +769,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -794,7 +786,9 @@
         <v>10</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
@@ -814,21 +808,11 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
         <v>10</v>
@@ -837,7 +821,7 @@
         <v>10</v>
       </c>
       <c r="J12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">

</xml_diff>